<commit_message>
Updated readme and PLO.
</commit_message>
<xml_diff>
--- a/common/PLOs.xlsx
+++ b/common/PLOs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/SPS Dropbox/Jason Bryer/Syllabi/common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2CE91B-7C7F-4147-89F9-22C30276B3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C08439-8C22-8048-8619-D2351E97B5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="11160" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{6D79DEB2-20F2-3B45-8B5E-87362AA71E0E}"/>
+    <workbookView xWindow="20600" yWindow="9160" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{6D79DEB2-20F2-3B45-8B5E-87362AA71E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="PLO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -207,18 +207,6 @@
     <t>IS 205 - IT Infrastructure and Support</t>
   </si>
   <si>
-    <t>IS 250 - Computer and Network Security</t>
-  </si>
-  <si>
-    <t>IS 260 - Networks and Business Data Comm</t>
-  </si>
-  <si>
-    <t>IS 305 - Cloud Computing</t>
-  </si>
-  <si>
-    <t>IS-321 - Device Security - Identity &amp; Access Mgt.</t>
-  </si>
-  <si>
     <t>IS-327- Security Operations</t>
   </si>
   <si>
@@ -337,6 +325,21 @@
   </si>
   <si>
     <t>IS360</t>
+  </si>
+  <si>
+    <t>General, Technical</t>
+  </si>
+  <si>
+    <t>IS361</t>
+  </si>
+  <si>
+    <t>Technical, Data Science</t>
+  </si>
+  <si>
+    <t>Technical, Cybersecurity</t>
+  </si>
+  <si>
+    <t>Foundational, Cybersecurity</t>
   </si>
 </sst>
 </file>
@@ -374,10 +377,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,94 +738,94 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B7:H7"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -830,17 +833,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12546C2C-1687-CA41-99C0-E0014542CC4F}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" style="2"/>
+    <col min="4" max="9" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -853,28 +856,28 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -882,22 +885,22 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
@@ -905,16 +908,16 @@
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -922,45 +925,45 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
@@ -968,48 +971,48 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -1017,19 +1020,19 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -1037,19 +1040,19 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -1057,19 +1060,19 @@
       <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -1077,19 +1080,19 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
@@ -1097,19 +1100,19 @@
       <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
@@ -1117,13 +1120,13 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
@@ -1131,13 +1134,13 @@
       <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
@@ -1145,13 +1148,13 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -1159,13 +1162,13 @@
       <c r="C16" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
@@ -1173,193 +1176,193 @@
       <c r="C17" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1371,16 +1374,16 @@
         <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1391,55 +1394,64 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1451,16 +1463,19 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1471,19 +1486,19 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1491,21 +1506,18 @@
         <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1514,22 +1526,19 @@
         <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>22</v>
+        <v>55</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1537,21 +1546,21 @@
         <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1560,21 +1569,21 @@
         <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1586,15 +1595,18 @@
         <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1606,193 +1618,18 @@
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I46" s="2" t="s">
+      <c r="D38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>